<commit_message>
Final Project, 3rd phase
</commit_message>
<xml_diff>
--- a/ContactFormData.xlsx
+++ b/ContactFormData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivana/Desktop/ITBootcamp/zavrsniPROJEKAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4A21D3-60A5-EE4A-8229-5623F2FC57AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166A4322-B050-4946-9D14-BA00DE0D35FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13880" yWindow="460" windowWidth="14540" windowHeight="16400" xr2:uid="{6B8ADFBC-BB9A-AB4F-84B4-C3103DEE62A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="47">
   <si>
     <t>SubjectHeading</t>
   </si>
@@ -157,13 +157,16 @@
     <t>20000000</t>
   </si>
   <si>
-    <t>marmoko@abc.com</t>
-  </si>
-  <si>
     <t>294053202</t>
   </si>
   <si>
     <t>Ne moze bez poruke</t>
+  </si>
+  <si>
+    <t>marmoko@ABC.COM</t>
+  </si>
+  <si>
+    <t>200000004</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -608,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -653,7 +656,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -894,7 +897,7 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>